<commit_message>
Change menu items order
</commit_message>
<xml_diff>
--- a/public/export.xlsx
+++ b/public/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Classement</t>
   </si>
@@ -35,16 +35,37 @@
     <t>Chronomètre</t>
   </si>
   <si>
+    <t>Ina AÏSSI</t>
+  </si>
+  <si>
+    <t>5 RIO GRANDE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>00:11:34</t>
+  </si>
+  <si>
+    <t>Robin BEAUFILS</t>
+  </si>
+  <si>
+    <t>5 AMAZONE</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
     <t>Shana AFFICHARD</t>
   </si>
   <si>
-    <t>5 RIO GRANDE</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>00:11:34</t>
+    <t>Yanis ALLIX</t>
+  </si>
+  <si>
+    <t>Thaïs BAILLARD</t>
+  </si>
+  <si>
+    <t>5 SANTA CRUZ</t>
   </si>
   <si>
     <t>Anna ANDREY</t>
@@ -387,7 +408,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,15 +464,95 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>